<commit_message>
evaluated 1.1A - 1.2B
</commit_message>
<xml_diff>
--- a/languageGP/test_problems/problem_1c.xlsx
+++ b/languageGP/test_problems/problem_1c.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="data.xlsx" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="data.xlsx" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,10 +426,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="n">
-        <v>1570228.928105155</v>
+        <v>7850.053870134598</v>
       </c>
       <c r="C1" t="n">
-        <v>1000</v>
+        <v>31.415</v>
       </c>
     </row>
     <row r="2">
@@ -437,10 +437,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>1426.399669728305</v>
+        <v>130.1127471719516</v>
       </c>
       <c r="C2" t="n">
-        <v>1000</v>
+        <v>28.2872894</v>
       </c>
     </row>
     <row r="3">
@@ -448,10 +448,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>1152.317</v>
+        <v>120.3434803475214</v>
       </c>
       <c r="C3" t="n">
-        <v>1000</v>
+        <v>28.2872894</v>
       </c>
     </row>
     <row r="4">
@@ -459,10 +459,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>1263.64567</v>
+        <v>29.90511544895237</v>
       </c>
       <c r="C4" t="n">
-        <v>1000</v>
+        <v>25.07504</v>
       </c>
     </row>
     <row r="5">
@@ -470,10 +470,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>46031.02118</v>
+        <v>567.0352436875779</v>
       </c>
       <c r="C5" t="n">
-        <v>1000</v>
+        <v>21.8446069</v>
       </c>
     </row>
     <row r="6">
@@ -481,10 +481,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>9877.419136999955</v>
+        <v>23.484465872</v>
       </c>
       <c r="C6" t="n">
-        <v>1000</v>
+        <v>19.4173051</v>
       </c>
     </row>
     <row r="7">
@@ -492,10 +492,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>40578.88494919825</v>
+        <v>23.958676206</v>
       </c>
       <c r="C7" t="n">
-        <v>1000</v>
+        <v>19.4173051</v>
       </c>
     </row>
     <row r="8">
@@ -503,10 +503,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>1747.39214</v>
+        <v>20.53691846200002</v>
       </c>
       <c r="C8" t="n">
-        <v>1000</v>
+        <v>18.9821576</v>
       </c>
     </row>
     <row r="9">
@@ -514,10 +514,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>40557.03056913448</v>
+        <v>39.21256949000001</v>
       </c>
       <c r="C9" t="n">
-        <v>1000</v>
+        <v>18.9561576</v>
       </c>
     </row>
     <row r="10">
@@ -525,10 +525,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>1423.3253589</v>
+        <v>19.88002691400001</v>
       </c>
       <c r="C10" t="n">
-        <v>1000</v>
+        <v>18.9561576</v>
       </c>
     </row>
     <row r="11">
@@ -536,10 +536,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>1128.119941</v>
+        <v>18.45777439999998</v>
       </c>
       <c r="C11" t="n">
-        <v>1000</v>
+        <v>18.0961176</v>
       </c>
     </row>
     <row r="12">
@@ -547,10 +547,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>1122.011342356324</v>
+        <v>17.94232312207999</v>
       </c>
       <c r="C12" t="n">
-        <v>1000</v>
+        <v>14.89492</v>
       </c>
     </row>
     <row r="13">
@@ -558,10 +558,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>14816.14861277196</v>
+        <v>15.73317475199999</v>
       </c>
       <c r="C13" t="n">
-        <v>1000</v>
+        <v>14.89492</v>
       </c>
     </row>
     <row r="14">
@@ -569,10 +569,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>32286.37261999937</v>
+        <v>15.37564619311711</v>
       </c>
       <c r="C14" t="n">
-        <v>1000</v>
+        <v>14.87593</v>
       </c>
     </row>
     <row r="15">
@@ -580,10 +580,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>1183.55146</v>
+        <v>15.32868840000001</v>
       </c>
       <c r="C15" t="n">
-        <v>1000</v>
+        <v>14.87593</v>
       </c>
     </row>
     <row r="16">
@@ -591,10 +591,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>14173.991</v>
+        <v>37.20487139999999</v>
       </c>
       <c r="C16" t="n">
-        <v>1000</v>
+        <v>14.87593</v>
       </c>
     </row>
     <row r="17">
@@ -602,10 +602,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>49394.50843000022</v>
+        <v>15.51132040000001</v>
       </c>
       <c r="C17" t="n">
-        <v>1000</v>
+        <v>14.87593</v>
       </c>
     </row>
     <row r="18">
@@ -613,10 +613,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>13835.1744158463</v>
+        <v>14.87593000000001</v>
       </c>
       <c r="C18" t="n">
-        <v>1000</v>
+        <v>14.87593</v>
       </c>
     </row>
     <row r="19">
@@ -624,10 +624,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>1180.31083</v>
+        <v>14.87593000000001</v>
       </c>
       <c r="C19" t="n">
-        <v>1000</v>
+        <v>14.87593</v>
       </c>
     </row>
     <row r="20">
@@ -635,10 +635,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>1092.12041</v>
+        <v>14.87593000000001</v>
       </c>
       <c r="C20" t="n">
-        <v>1000</v>
+        <v>14.87593</v>
       </c>
     </row>
     <row r="21">
@@ -646,10 +646,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>13520.31229019675</v>
+        <v>14.87593000000001</v>
       </c>
       <c r="C21" t="n">
-        <v>1000</v>
+        <v>14.87593</v>
       </c>
     </row>
     <row r="22">
@@ -657,10 +657,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>1091.69838</v>
+        <v>15.79032778400001</v>
       </c>
       <c r="C22" t="n">
-        <v>1000</v>
+        <v>14.87593</v>
       </c>
     </row>
     <row r="23">
@@ -668,10 +668,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>1091.566</v>
+        <v>14.87593000000001</v>
       </c>
       <c r="C23" t="n">
-        <v>1000</v>
+        <v>14.87593</v>
       </c>
     </row>
     <row r="24">
@@ -679,10 +679,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>15414.47404</v>
+        <v>15.42782454400001</v>
       </c>
       <c r="C24" t="n">
-        <v>1000</v>
+        <v>14.87593</v>
       </c>
     </row>
     <row r="25">
@@ -690,10 +690,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>1061.46617</v>
+        <v>14.87593000000001</v>
       </c>
       <c r="C25" t="n">
-        <v>1000</v>
+        <v>14.87593</v>
       </c>
     </row>
     <row r="26">
@@ -701,10 +701,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>40374.83482655897</v>
+        <v>14.8220316</v>
       </c>
       <c r="C26" t="n">
-        <v>1000</v>
+        <v>14.25293</v>
       </c>
     </row>
     <row r="27">
@@ -712,10 +712,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>32380.088</v>
+        <v>9.517035799999991</v>
       </c>
       <c r="C27" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="28">
@@ -723,10 +723,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>1152.275</v>
+        <v>2.880952199999999</v>
       </c>
       <c r="C28" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="29">
@@ -734,10 +734,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>1121.6548</v>
+        <v>1.68856</v>
       </c>
       <c r="C29" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="30">
@@ -745,10 +745,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>1121.738</v>
+        <v>2.94824</v>
       </c>
       <c r="C30" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="31">
@@ -756,10 +756,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>1030.34077</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C31" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="32">
@@ -767,10 +767,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>25277.616</v>
+        <v>191.3824917559504</v>
       </c>
       <c r="C32" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="33">
@@ -778,10 +778,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>1091.199602532781</v>
+        <v>1205.975823590102</v>
       </c>
       <c r="C33" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="34">
@@ -789,10 +789,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>1030.38568</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C34" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="35">
@@ -800,10 +800,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>1182.671431052427</v>
+        <v>2.312599999999999</v>
       </c>
       <c r="C35" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="36">
@@ -811,10 +811,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>63889.03128</v>
+        <v>2.722422000000001</v>
       </c>
       <c r="C36" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="37">
@@ -822,10 +822,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>1030.53837</v>
+        <v>2.710400000000001</v>
       </c>
       <c r="C37" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="38">
@@ -833,10 +833,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>1030.615</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C38" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="39">
@@ -844,10 +844,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>1030.915</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C39" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="40">
@@ -855,10 +855,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>1030.43837</v>
+        <v>1.365599999999999</v>
       </c>
       <c r="C40" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="41">
@@ -866,10 +866,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>1122.04419</v>
+        <v>1.1592</v>
       </c>
       <c r="C41" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="42">
@@ -877,10 +877,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>1030.64326</v>
+        <v>352.2422000000013</v>
       </c>
       <c r="C42" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="43">
@@ -888,10 +888,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>1030.75301</v>
+        <v>1.2624</v>
       </c>
       <c r="C43" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="44">
@@ -899,10 +899,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>1030.49606</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C44" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="45">
@@ -910,10 +910,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>1121.98112</v>
+        <v>1.074199999999999</v>
       </c>
       <c r="C45" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="46">
@@ -921,10 +921,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>1030.679</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C46" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="47">
@@ -932,10 +932,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>49515.76828000044</v>
+        <v>6.472656</v>
       </c>
       <c r="C47" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="48">
@@ -943,10 +943,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>1117.2414384</v>
+        <v>1.426251999999999</v>
       </c>
       <c r="C48" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="49">
@@ -954,10 +954,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>1060.775</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C49" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="50">
@@ -965,10 +965,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>1061.13</v>
+        <v>21.02581199999999</v>
       </c>
       <c r="C50" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="51">
@@ -976,10 +976,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>1090.41524</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C51" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="52">
@@ -987,10 +987,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>70749.29281000106</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C52" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="53">
@@ -998,10 +998,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>40407.54865999999</v>
+        <v>1.074079999999999</v>
       </c>
       <c r="C53" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="54">
@@ -1009,10 +1009,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>1122.558</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C54" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="55">
@@ -1020,10 +1020,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>17748.89833</v>
+        <v>2.334026799999999</v>
       </c>
       <c r="C55" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="56">
@@ -1031,10 +1031,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="n">
-        <v>36017.58491</v>
+        <v>1.083299999999999</v>
       </c>
       <c r="C56" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="57">
@@ -1042,10 +1042,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="n">
-        <v>1091.59357</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C57" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="58">
@@ -1053,10 +1053,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>84014.17101000175</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C58" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="59">
@@ -1064,10 +1064,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>1092.26137</v>
+        <v>1.2288</v>
       </c>
       <c r="C59" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="60">
@@ -1075,10 +1075,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>1061.064</v>
+        <v>1.082499999999999</v>
       </c>
       <c r="C60" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="61">
@@ -1086,10 +1086,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>1061.2213125</v>
+        <v>834.5195512000116</v>
       </c>
       <c r="C61" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="62">
@@ -1097,10 +1097,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="n">
-        <v>1061.23</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C62" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="63">
@@ -1108,10 +1108,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="n">
-        <v>1091.25527</v>
+        <v>0.9243019999999995</v>
       </c>
       <c r="C63" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="64">
@@ -1119,10 +1119,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="n">
-        <v>1030.626</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C64" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="65">
@@ -1130,10 +1130,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="n">
-        <v>1203.83</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C65" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="66">
@@ -1141,10 +1141,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="n">
-        <v>1030.64747</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C66" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="67">
@@ -1152,10 +1152,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="n">
-        <v>18487.96604</v>
+        <v>1.081598599999999</v>
       </c>
       <c r="C67" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="68">
@@ -1163,10 +1163,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="n">
-        <v>1030.61726</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C68" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="69">
@@ -1174,10 +1174,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="n">
-        <v>1121.64847</v>
+        <v>1.700725956175125</v>
       </c>
       <c r="C69" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="70">
@@ -1185,10 +1185,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="n">
-        <v>14726.3115568</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C70" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="71">
@@ -1196,10 +1196,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="n">
-        <v>18495.31821</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C71" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="72">
@@ -1207,10 +1207,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="n">
-        <v>1121.59207</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C72" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="73">
@@ -1218,10 +1218,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="n">
-        <v>1122.18809680662</v>
+        <v>1.083259999999999</v>
       </c>
       <c r="C73" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="74">
@@ -1229,10 +1229,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="n">
-        <v>1030.615</v>
+        <v>1.074199999999999</v>
       </c>
       <c r="C74" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="75">
@@ -1240,10 +1240,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="n">
-        <v>1122.93791</v>
+        <v>1.02956</v>
       </c>
       <c r="C75" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="76">
@@ -1251,10 +1251,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="n">
-        <v>1230.46521</v>
+        <v>411.5623399999992</v>
       </c>
       <c r="C76" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="77">
@@ -1262,10 +1262,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="n">
-        <v>1143.1</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C77" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="78">
@@ -1273,10 +1273,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="n">
-        <v>1091.73869</v>
+        <v>1.0742</v>
       </c>
       <c r="C78" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="79">
@@ -1284,10 +1284,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="n">
-        <v>1091.445</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C79" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="80">
@@ -1295,10 +1295,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="n">
-        <v>40324.48402000011</v>
+        <v>1.0742</v>
       </c>
       <c r="C80" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="81">
@@ -1306,10 +1306,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="n">
-        <v>1091.594</v>
+        <v>3.081944200000003</v>
       </c>
       <c r="C81" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="82">
@@ -1317,10 +1317,10 @@
         <v>81</v>
       </c>
       <c r="B82" t="n">
-        <v>1061.06147</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C82" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="83">
@@ -1328,10 +1328,10 @@
         <v>82</v>
       </c>
       <c r="B83" t="n">
-        <v>1250.46065</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C83" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="84">
@@ -1339,10 +1339,10 @@
         <v>83</v>
       </c>
       <c r="B84" t="n">
-        <v>1231.1287272</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C84" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="85">
@@ -1350,10 +1350,10 @@
         <v>84</v>
       </c>
       <c r="B85" t="n">
-        <v>53351.26344999877</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C85" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="86">
@@ -1361,10 +1361,10 @@
         <v>85</v>
       </c>
       <c r="B86" t="n">
-        <v>1173.27086</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C86" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="87">
@@ -1372,10 +1372,10 @@
         <v>86</v>
       </c>
       <c r="B87" t="n">
-        <v>1091.30551</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C87" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="88">
@@ -1383,10 +1383,10 @@
         <v>87</v>
       </c>
       <c r="B88" t="n">
-        <v>40437.974</v>
+        <v>1.0724232</v>
       </c>
       <c r="C88" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="89">
@@ -1394,10 +1394,10 @@
         <v>88</v>
       </c>
       <c r="B89" t="n">
-        <v>1031.128</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C89" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="90">
@@ -1405,10 +1405,10 @@
         <v>89</v>
       </c>
       <c r="B90" t="n">
-        <v>15999.00495000015</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C90" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="91">
@@ -1416,10 +1416,10 @@
         <v>90</v>
       </c>
       <c r="B91" t="n">
-        <v>1030.615</v>
+        <v>1.708785799999999</v>
       </c>
       <c r="C91" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="92">
@@ -1427,10 +1427,10 @@
         <v>91</v>
       </c>
       <c r="B92" t="n">
-        <v>1030.457</v>
+        <v>1.0742</v>
       </c>
       <c r="C92" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="93">
@@ -1438,10 +1438,10 @@
         <v>92</v>
       </c>
       <c r="B93" t="n">
-        <v>1030.535</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C93" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="94">
@@ -1449,10 +1449,10 @@
         <v>93</v>
       </c>
       <c r="B94" t="n">
-        <v>1121.74699</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C94" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="95">
@@ -1460,10 +1460,10 @@
         <v>94</v>
       </c>
       <c r="B95" t="n">
-        <v>1182.390381771103</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C95" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="96">
@@ -1471,10 +1471,10 @@
         <v>95</v>
       </c>
       <c r="B96" t="n">
-        <v>1091.719</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C96" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="97">
@@ -1482,10 +1482,10 @@
         <v>96</v>
       </c>
       <c r="B97" t="n">
-        <v>1030.615</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C97" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="98">
@@ -1493,10 +1493,10 @@
         <v>97</v>
       </c>
       <c r="B98" t="n">
-        <v>37980.596</v>
+        <v>40.58953599999999</v>
       </c>
       <c r="C98" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="99">
@@ -1504,10 +1504,10 @@
         <v>98</v>
       </c>
       <c r="B99" t="n">
-        <v>1061.191356896552</v>
+        <v>1.0741</v>
       </c>
       <c r="C99" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="100">
@@ -1515,10 +1515,10 @@
         <v>99</v>
       </c>
       <c r="B100" t="n">
-        <v>32379.65303</v>
+        <v>20.4459</v>
       </c>
       <c r="C100" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="101">
@@ -1526,10 +1526,10 @@
         <v>100</v>
       </c>
       <c r="B101" t="n">
-        <v>825804.182924925</v>
+        <v>3.0833</v>
       </c>
       <c r="C101" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="102">
@@ -1537,10 +1537,10 @@
         <v>101</v>
       </c>
       <c r="B102" t="n">
-        <v>1152.23705</v>
+        <v>2.455</v>
       </c>
       <c r="C102" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="103">
@@ -1548,10 +1548,10 @@
         <v>102</v>
       </c>
       <c r="B103" t="n">
-        <v>1092.03584</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C103" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="104">
@@ -1559,10 +1559,10 @@
         <v>103</v>
       </c>
       <c r="B104" t="n">
-        <v>1091.74541</v>
+        <v>20.44590000000001</v>
       </c>
       <c r="C104" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="105">
@@ -1570,10 +1570,10 @@
         <v>104</v>
       </c>
       <c r="B105" t="n">
-        <v>1061.1606</v>
+        <v>1.083299999999999</v>
       </c>
       <c r="C105" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="106">
@@ -1581,10 +1581,10 @@
         <v>105</v>
       </c>
       <c r="B106" t="n">
-        <v>1030.615</v>
+        <v>20.44590000000002</v>
       </c>
       <c r="C106" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="107">
@@ -1592,10 +1592,10 @@
         <v>106</v>
       </c>
       <c r="B107" t="n">
-        <v>1030.38289</v>
+        <v>1.184356</v>
       </c>
       <c r="C107" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="108">
@@ -1603,10 +1603,10 @@
         <v>107</v>
       </c>
       <c r="B108" t="n">
-        <v>1091.63458</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C108" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="109">
@@ -1614,10 +1614,10 @@
         <v>108</v>
       </c>
       <c r="B109" t="n">
-        <v>1030.589</v>
+        <v>1.0742</v>
       </c>
       <c r="C109" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="110">
@@ -1625,10 +1625,10 @@
         <v>109</v>
       </c>
       <c r="B110" t="n">
-        <v>38851.66919999993</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C110" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="111">
@@ -1636,10 +1636,10 @@
         <v>110</v>
       </c>
       <c r="B111" t="n">
-        <v>1122.22103</v>
+        <v>906.6435999999911</v>
       </c>
       <c r="C111" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="112">
@@ -1647,10 +1647,10 @@
         <v>111</v>
       </c>
       <c r="B112" t="n">
-        <v>1060.964</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C112" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="113">
@@ -1658,10 +1658,10 @@
         <v>112</v>
       </c>
       <c r="B113" t="n">
-        <v>1091.19222</v>
+        <v>1.642405055999999</v>
       </c>
       <c r="C113" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="114">
@@ -1669,10 +1669,10 @@
         <v>113</v>
       </c>
       <c r="B114" t="n">
-        <v>1030.6793</v>
+        <v>2.455</v>
       </c>
       <c r="C114" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="115">
@@ -1680,10 +1680,10 @@
         <v>114</v>
       </c>
       <c r="B115" t="n">
-        <v>1121.823269558824</v>
+        <v>20.4459</v>
       </c>
       <c r="C115" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="116">
@@ -1691,10 +1691,10 @@
         <v>115</v>
       </c>
       <c r="B116" t="n">
-        <v>1369.0845788</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C116" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="117">
@@ -1702,10 +1702,10 @@
         <v>116</v>
       </c>
       <c r="B117" t="n">
-        <v>1152.19279</v>
+        <v>2.220052799999999</v>
       </c>
       <c r="C117" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="118">
@@ -1713,10 +1713,10 @@
         <v>117</v>
       </c>
       <c r="B118" t="n">
-        <v>1061.22081</v>
+        <v>2.499524799999999</v>
       </c>
       <c r="C118" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="119">
@@ -1724,10 +1724,10 @@
         <v>118</v>
       </c>
       <c r="B119" t="n">
-        <v>1061.266</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C119" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="120">
@@ -1735,10 +1735,10 @@
         <v>119</v>
       </c>
       <c r="B120" t="n">
-        <v>46033.67956000078</v>
+        <v>1.0742</v>
       </c>
       <c r="C120" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="121">
@@ -1746,10 +1746,10 @@
         <v>120</v>
       </c>
       <c r="B121" t="n">
-        <v>20728.407</v>
+        <v>1841.0730054</v>
       </c>
       <c r="C121" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="122">
@@ -1757,10 +1757,10 @@
         <v>121</v>
       </c>
       <c r="B122" t="n">
-        <v>1061.06433</v>
+        <v>1.0742</v>
       </c>
       <c r="C122" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="123">
@@ -1768,10 +1768,10 @@
         <v>122</v>
       </c>
       <c r="B123" t="n">
-        <v>1030.615</v>
+        <v>1.587996</v>
       </c>
       <c r="C123" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="124">
@@ -1779,10 +1779,10 @@
         <v>123</v>
       </c>
       <c r="B124" t="n">
-        <v>1152.23731</v>
+        <v>1.08194</v>
       </c>
       <c r="C124" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="125">
@@ -1790,10 +1790,10 @@
         <v>124</v>
       </c>
       <c r="B125" t="n">
-        <v>1061.88561</v>
+        <v>5.418426800000001</v>
       </c>
       <c r="C125" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="126">
@@ -1801,10 +1801,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="n">
-        <v>1143.1</v>
+        <v>3.7000258</v>
       </c>
       <c r="C126" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="127">
@@ -1812,10 +1812,10 @@
         <v>126</v>
       </c>
       <c r="B127" t="n">
-        <v>15350.85633000013</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C127" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="128">
@@ -1823,10 +1823,10 @@
         <v>127</v>
       </c>
       <c r="B128" t="n">
-        <v>58254.09879</v>
+        <v>2.455</v>
       </c>
       <c r="C128" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="129">
@@ -1834,10 +1834,10 @@
         <v>128</v>
       </c>
       <c r="B129" t="n">
-        <v>1152.02674</v>
+        <v>2.455</v>
       </c>
       <c r="C129" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="130">
@@ -1845,10 +1845,10 @@
         <v>129</v>
       </c>
       <c r="B130" t="n">
-        <v>40173.1377299998</v>
+        <v>0.4549999999999995</v>
       </c>
       <c r="C130" t="n">
-        <v>1000</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="131">
@@ -1856,10 +1856,10 @@
         <v>130</v>
       </c>
       <c r="B131" t="n">
-        <v>1122.70529</v>
+        <v>1.668609599999999</v>
       </c>
       <c r="C131" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="132">
@@ -1867,10 +1867,10 @@
         <v>131</v>
       </c>
       <c r="B132" t="n">
-        <v>1061.142</v>
+        <v>0.3106000000000003</v>
       </c>
       <c r="C132" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="133">
@@ -1878,10 +1878,10 @@
         <v>132</v>
       </c>
       <c r="B133" t="n">
-        <v>1091.63267</v>
+        <v>1.0584768</v>
       </c>
       <c r="C133" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="134">
@@ -1889,10 +1889,10 @@
         <v>133</v>
       </c>
       <c r="B134" t="n">
-        <v>20685.48524000004</v>
+        <v>1684.9883</v>
       </c>
       <c r="C134" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="135">
@@ -1900,10 +1900,10 @@
         <v>134</v>
       </c>
       <c r="B135" t="n">
-        <v>1158.120783333333</v>
+        <v>0.7728000000000002</v>
       </c>
       <c r="C135" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="136">
@@ -1911,10 +1911,10 @@
         <v>135</v>
       </c>
       <c r="B136" t="n">
-        <v>1174.08441</v>
+        <v>20.8827</v>
       </c>
       <c r="C136" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="137">
@@ -1922,10 +1922,10 @@
         <v>136</v>
       </c>
       <c r="B137" t="n">
-        <v>71024.63689999914</v>
+        <v>1558.2597</v>
       </c>
       <c r="C137" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="138">
@@ -1933,10 +1933,10 @@
         <v>137</v>
       </c>
       <c r="B138" t="n">
-        <v>1121.68266</v>
+        <v>524.5635403999928</v>
       </c>
       <c r="C138" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="139">
@@ -1944,10 +1944,10 @@
         <v>138</v>
       </c>
       <c r="B139" t="n">
-        <v>77470.65374009204</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C139" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="140">
@@ -1955,10 +1955,10 @@
         <v>139</v>
       </c>
       <c r="B140" t="n">
-        <v>42559.236227</v>
+        <v>169.5984079999995</v>
       </c>
       <c r="C140" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="141">
@@ -1966,10 +1966,10 @@
         <v>140</v>
       </c>
       <c r="B141" t="n">
-        <v>1212.67827</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C141" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="142">
@@ -1977,10 +1977,10 @@
         <v>141</v>
       </c>
       <c r="B142" t="n">
-        <v>1061.001</v>
+        <v>3.24174</v>
       </c>
       <c r="C142" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="143">
@@ -1988,10 +1988,10 @@
         <v>142</v>
       </c>
       <c r="B143" t="n">
-        <v>1030.715</v>
+        <v>2.265</v>
       </c>
       <c r="C143" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="144">
@@ -1999,10 +1999,10 @@
         <v>143</v>
       </c>
       <c r="B144" t="n">
-        <v>1158.10216</v>
+        <v>0.8879921023534988</v>
       </c>
       <c r="C144" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="145">
@@ -2010,10 +2010,10 @@
         <v>144</v>
       </c>
       <c r="B145" t="n">
-        <v>1056.01495</v>
+        <v>0.8635824000000001</v>
       </c>
       <c r="C145" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="146">
@@ -2021,10 +2021,10 @@
         <v>145</v>
       </c>
       <c r="B146" t="n">
-        <v>1213.28207</v>
+        <v>0.5098000000000001</v>
       </c>
       <c r="C146" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="147">
@@ -2032,10 +2032,10 @@
         <v>146</v>
       </c>
       <c r="B147" t="n">
-        <v>37987.84291999988</v>
+        <v>0.8880000000000001</v>
       </c>
       <c r="C147" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="148">
@@ -2043,10 +2043,10 @@
         <v>147</v>
       </c>
       <c r="B148" t="n">
-        <v>20611.32900000022</v>
+        <v>1049.402541599974</v>
       </c>
       <c r="C148" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="149">
@@ -2054,10 +2054,10 @@
         <v>148</v>
       </c>
       <c r="B149" t="n">
-        <v>1060.8284</v>
+        <v>0.8880000000000001</v>
       </c>
       <c r="C149" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="150">
@@ -2065,10 +2065,10 @@
         <v>149</v>
       </c>
       <c r="B150" t="n">
-        <v>1060.938</v>
+        <v>2.867168399999999</v>
       </c>
       <c r="C150" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="151">
@@ -2076,10 +2076,10 @@
         <v>150</v>
       </c>
       <c r="B151" t="n">
-        <v>20667.86949</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C151" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="152">
@@ -2087,10 +2087,10 @@
         <v>151</v>
       </c>
       <c r="B152" t="n">
-        <v>1086.015</v>
+        <v>2.265</v>
       </c>
       <c r="C152" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="153">
@@ -2098,10 +2098,10 @@
         <v>152</v>
       </c>
       <c r="B153" t="n">
-        <v>1061.03</v>
+        <v>0.8880000000000001</v>
       </c>
       <c r="C153" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="154">
@@ -2109,10 +2109,10 @@
         <v>153</v>
       </c>
       <c r="B154" t="n">
-        <v>36281.5827600004</v>
+        <v>0.8880000000000001</v>
       </c>
       <c r="C154" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="155">
@@ -2120,10 +2120,10 @@
         <v>154</v>
       </c>
       <c r="B155" t="n">
-        <v>1091.301</v>
+        <v>0.6833472</v>
       </c>
       <c r="C155" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="156">
@@ -2131,10 +2131,10 @@
         <v>155</v>
       </c>
       <c r="B156" t="n">
-        <v>35997.95731000075</v>
+        <v>3.51629892716206</v>
       </c>
       <c r="C156" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="157">
@@ -2142,10 +2142,10 @@
         <v>156</v>
       </c>
       <c r="B157" t="n">
-        <v>1121.74843</v>
+        <v>1.4784</v>
       </c>
       <c r="C157" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="158">
@@ -2153,10 +2153,10 @@
         <v>157</v>
       </c>
       <c r="B158" t="n">
-        <v>1030.55435</v>
+        <v>0.8874400000000001</v>
       </c>
       <c r="C158" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="159">
@@ -2164,10 +2164,10 @@
         <v>158</v>
       </c>
       <c r="B159" t="n">
-        <v>1266.9</v>
+        <v>0.8874026206896554</v>
       </c>
       <c r="C159" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="160">
@@ -2175,10 +2175,10 @@
         <v>159</v>
       </c>
       <c r="B160" t="n">
-        <v>1321.73152</v>
+        <v>1.5195346</v>
       </c>
       <c r="C160" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="161">
@@ -2186,10 +2186,10 @@
         <v>160</v>
       </c>
       <c r="B161" t="n">
-        <v>15370.52149999992</v>
+        <v>656.2597000000001</v>
       </c>
       <c r="C161" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="162">
@@ -2197,10 +2197,10 @@
         <v>161</v>
       </c>
       <c r="B162" t="n">
-        <v>1424.97281755102</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C162" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="163">
@@ -2208,10 +2208,10 @@
         <v>162</v>
       </c>
       <c r="B163" t="n">
-        <v>46055.397</v>
+        <v>0.3365568000000002</v>
       </c>
       <c r="C163" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="164">
@@ -2219,10 +2219,10 @@
         <v>163</v>
       </c>
       <c r="B164" t="n">
-        <v>1185.66062</v>
+        <v>0.8922106000000001</v>
       </c>
       <c r="C164" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="165">
@@ -2230,10 +2230,10 @@
         <v>164</v>
       </c>
       <c r="B165" t="n">
-        <v>1092.34241</v>
+        <v>1127.250496000004</v>
       </c>
       <c r="C165" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="166">
@@ -2241,10 +2241,10 @@
         <v>165</v>
       </c>
       <c r="B166" t="n">
-        <v>35946.31679999975</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C166" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="167">
@@ -2252,10 +2252,10 @@
         <v>166</v>
       </c>
       <c r="B167" t="n">
-        <v>1110.8</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C167" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="168">
@@ -2263,10 +2263,10 @@
         <v>167</v>
       </c>
       <c r="B168" t="n">
-        <v>32321.25224000066</v>
+        <v>1.1328</v>
       </c>
       <c r="C168" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="169">
@@ -2274,10 +2274,10 @@
         <v>168</v>
       </c>
       <c r="B169" t="n">
-        <v>11919.12820000002</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C169" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="170">
@@ -2285,10 +2285,10 @@
         <v>169</v>
       </c>
       <c r="B170" t="n">
-        <v>1121.917</v>
+        <v>20.2597</v>
       </c>
       <c r="C170" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="171">
@@ -2296,10 +2296,10 @@
         <v>170</v>
       </c>
       <c r="B171" t="n">
-        <v>1060.97132</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C171" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="172">
@@ -2307,10 +2307,10 @@
         <v>171</v>
       </c>
       <c r="B172" t="n">
-        <v>1047.8</v>
+        <v>22.88270000000003</v>
       </c>
       <c r="C172" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="173">
@@ -2318,10 +2318,10 @@
         <v>172</v>
       </c>
       <c r="B173" t="n">
-        <v>1092.7322</v>
+        <v>4.187448</v>
       </c>
       <c r="C173" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="174">
@@ -2329,10 +2329,10 @@
         <v>173</v>
       </c>
       <c r="B174" t="n">
-        <v>1030.615532608696</v>
+        <v>20.2597</v>
       </c>
       <c r="C174" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="175">
@@ -2340,10 +2340,10 @@
         <v>174</v>
       </c>
       <c r="B175" t="n">
-        <v>1121.80573</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C175" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="176">
@@ -2351,10 +2351,10 @@
         <v>175</v>
       </c>
       <c r="B176" t="n">
-        <v>1058.04135</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C176" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="177">
@@ -2362,10 +2362,10 @@
         <v>176</v>
       </c>
       <c r="B177" t="n">
-        <v>1181.78017</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C177" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="178">
@@ -2373,10 +2373,10 @@
         <v>177</v>
       </c>
       <c r="B178" t="n">
-        <v>1060.93</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C178" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="179">
@@ -2384,10 +2384,10 @@
         <v>178</v>
       </c>
       <c r="B179" t="n">
-        <v>1030.63117</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C179" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="180">
@@ -2395,10 +2395,10 @@
         <v>179</v>
       </c>
       <c r="B180" t="n">
-        <v>1060.787960482375</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C180" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="181">
@@ -2406,10 +2406,10 @@
         <v>180</v>
       </c>
       <c r="B181" t="n">
-        <v>15248.0232000001</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C181" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="182">
@@ -2417,10 +2417,10 @@
         <v>181</v>
       </c>
       <c r="B182" t="n">
-        <v>63875.7234400011</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C182" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="183">
@@ -2428,10 +2428,10 @@
         <v>182</v>
       </c>
       <c r="B183" t="n">
-        <v>1030.613</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C183" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="184">
@@ -2439,10 +2439,10 @@
         <v>183</v>
       </c>
       <c r="B184" t="n">
-        <v>1030.515</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C184" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="185">
@@ -2450,10 +2450,10 @@
         <v>184</v>
       </c>
       <c r="B185" t="n">
-        <v>1273.474989125252</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C185" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="186">
@@ -2461,10 +2461,10 @@
         <v>185</v>
       </c>
       <c r="B186" t="n">
-        <v>1091.5119</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C186" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="187">
@@ -2472,10 +2472,10 @@
         <v>186</v>
       </c>
       <c r="B187" t="n">
-        <v>1092.745</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C187" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="188">
@@ -2483,10 +2483,10 @@
         <v>187</v>
       </c>
       <c r="B188" t="n">
-        <v>1058.9</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C188" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="189">
@@ -2494,10 +2494,10 @@
         <v>188</v>
       </c>
       <c r="B189" t="n">
-        <v>1060.936</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C189" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="190">
@@ -2505,10 +2505,10 @@
         <v>189</v>
       </c>
       <c r="B190" t="n">
-        <v>40319.57954999999</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C190" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="191">
@@ -2516,10 +2516,10 @@
         <v>190</v>
       </c>
       <c r="B191" t="n">
-        <v>1063.52105</v>
+        <v>0.8625600000000001</v>
       </c>
       <c r="C191" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="192">
@@ -2527,10 +2527,10 @@
         <v>191</v>
       </c>
       <c r="B192" t="n">
-        <v>15346.34670999987</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C192" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="193">
@@ -2538,10 +2538,10 @@
         <v>192</v>
       </c>
       <c r="B193" t="n">
-        <v>19682.34283</v>
+        <v>1.712208</v>
       </c>
       <c r="C193" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="194">
@@ -2549,10 +2549,10 @@
         <v>193</v>
       </c>
       <c r="B194" t="n">
-        <v>1112.173704</v>
+        <v>1.5227754</v>
       </c>
       <c r="C194" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="195">
@@ -2560,10 +2560,10 @@
         <v>194</v>
       </c>
       <c r="B195" t="n">
-        <v>1061.028914027149</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C195" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="196">
@@ -2571,10 +2571,10 @@
         <v>195</v>
       </c>
       <c r="B196" t="n">
-        <v>22018.698</v>
+        <v>676.2596999999998</v>
       </c>
       <c r="C196" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="197">
@@ -2582,10 +2582,10 @@
         <v>196</v>
       </c>
       <c r="B197" t="n">
-        <v>1091.438884210526</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C197" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="198">
@@ -2593,10 +2593,10 @@
         <v>197</v>
       </c>
       <c r="B198" t="n">
-        <v>79577.85405999867</v>
+        <v>0.2650000000000001</v>
       </c>
       <c r="C198" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="199">
@@ -2604,10 +2604,10 @@
         <v>198</v>
       </c>
       <c r="B199" t="n">
-        <v>1061.21385</v>
+        <v>1.24938</v>
       </c>
       <c r="C199" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="200">
@@ -2615,10 +2615,10 @@
         <v>199</v>
       </c>
       <c r="B200" t="n">
-        <v>1061.186</v>
+        <v>1.510718342509418</v>
       </c>
       <c r="C200" t="n">
-        <v>1000</v>
+        <v>0.265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>